<commit_message>
Corrects note on reverb transformer, link for inductor
</commit_message>
<xml_diff>
--- a/BOM/Europe/non-mouser-BOM.xlsx
+++ b/BOM/Europe/non-mouser-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/dev/git/timrobertson100/steel-string-singer-sn-002/BOM/Europe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854090F0-92E2-3645-A154-B17CB3001F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC450B47-1E6E-2546-B4BF-3D90C6BBD84C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7640" yWindow="6500" windowWidth="29040" windowHeight="15840" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="139">
   <si>
     <t>UOM</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>ha1750b</t>
-  </si>
-  <si>
-    <t>1750a may be suitable, and cheaper?</t>
   </si>
   <si>
     <t>SKU 23429</t>
@@ -470,11 +467,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -565,14 +561,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0066CC"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF6600"/>
       <name val="Calibri"/>
@@ -607,14 +595,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -634,11 +621,10 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -956,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBE67D0-6312-A44B-85E3-458F1293B8D9}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,11 +961,11 @@
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="D1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -994,107 +980,107 @@
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+    <row r="4" spans="1:7" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>2.33</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <f t="shared" ref="F4:F49" si="0">A4*E4</f>
         <v>2.33</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="12">
+        <v>3.75</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="G5" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="13">
-        <v>3.75</v>
-      </c>
-      <c r="F5" s="13">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>10</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
         <v>91</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="F6" s="13">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>0.3</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1110,10 +1096,10 @@
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>2.75</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
@@ -1131,10 +1117,10 @@
       <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>2.75</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <f t="shared" si="0"/>
         <v>8.25</v>
       </c>
@@ -1152,10 +1138,10 @@
       <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>2.75</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
@@ -1173,10 +1159,10 @@
       <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>2.92</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <f t="shared" si="0"/>
         <v>2.92</v>
       </c>
@@ -1194,10 +1180,10 @@
       <c r="D12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <v>3.57</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <f t="shared" si="0"/>
         <v>3.57</v>
       </c>
@@ -1215,10 +1201,10 @@
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>0.4</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
@@ -1239,10 +1225,10 @@
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>1.48</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <f t="shared" si="0"/>
         <v>10.36</v>
       </c>
@@ -1260,10 +1246,10 @@
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>1.48</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
         <f t="shared" si="0"/>
         <v>4.4399999999999995</v>
       </c>
@@ -1281,15 +1267,15 @@
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>1.24</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
       <c r="G16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1305,10 +1291,10 @@
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>1.95</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <f t="shared" ref="F17" si="1">A17*E17</f>
         <v>11.7</v>
       </c>
@@ -1326,10 +1312,10 @@
       <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>1.89</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
@@ -1347,10 +1333,10 @@
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>1.17</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
@@ -1368,10 +1354,10 @@
       <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>4.08</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f t="shared" si="0"/>
         <v>4.08</v>
       </c>
@@ -1392,10 +1378,10 @@
       <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>4.63</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <f t="shared" si="0"/>
         <v>9.26</v>
       </c>
@@ -1413,10 +1399,10 @@
       <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <v>3.93</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <f t="shared" si="0"/>
         <v>7.86</v>
       </c>
@@ -1434,40 +1420,40 @@
       <c r="D23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>3.14</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <f t="shared" si="0"/>
         <v>9.42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="19">
+    <row r="24" spans="1:7" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
         <v>1</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="20" t="s">
+      <c r="B24" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <v>26.41</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <f t="shared" si="0"/>
         <v>26.41</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>90</v>
+      <c r="G24" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="8">
+      <c r="A25" s="7">
         <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1479,19 +1465,19 @@
       <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <v>2.3199999999999998</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="12">
         <f t="shared" si="0"/>
         <v>13.919999999999998</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>121</v>
+      <c r="G25" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
+      <c r="A26" s="8">
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1503,10 +1489,10 @@
       <c r="D26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <v>5</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1515,27 +1501,27 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="20" t="s">
+      <c r="B27" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="E27" s="20">
+        <v>11.84</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="0"/>
+        <v>11.84</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>89</v>
-      </c>
-      <c r="E27" s="21">
-        <v>11.84</v>
-      </c>
-      <c r="F27" s="21">
-        <f t="shared" si="0"/>
-        <v>11.84</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1551,10 +1537,10 @@
       <c r="D28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>2.86</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="12">
         <f t="shared" si="0"/>
         <v>8.58</v>
       </c>
@@ -1572,16 +1558,16 @@
       <c r="D29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <v>2.25</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="12">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="8">
+      <c r="A30" s="7">
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1593,36 +1579,36 @@
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>2.33</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="12">
         <f t="shared" si="0"/>
         <v>4.66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="19">
+    <row r="31" spans="1:7" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="18">
         <v>2</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="20" t="s">
+      <c r="B31" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="20">
         <v>2.5099999999999998</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="20">
         <f t="shared" si="0"/>
         <v>5.0199999999999996</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>90</v>
+      <c r="G31" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1638,10 +1624,10 @@
       <c r="D32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <v>49.9</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="12">
         <f t="shared" si="0"/>
         <v>49.9</v>
       </c>
@@ -1654,212 +1640,212 @@
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="13">
+        <v>106</v>
+      </c>
+      <c r="E33" s="12">
         <v>0.48</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="20">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>104</v>
+      <c r="G33" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="19">
+      <c r="A34" s="18">
         <v>50</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="20" t="s">
+      <c r="B34" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="20">
+        <v>0.13</v>
+      </c>
+      <c r="F34" s="20">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="18">
+        <v>50</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="21">
-        <v>0.13</v>
-      </c>
-      <c r="F34" s="21">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="19">
-        <v>50</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="20" t="s">
+      <c r="E35" s="20">
+        <v>0.12</v>
+      </c>
+      <c r="F35" s="20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G35" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="21">
-        <v>0.12</v>
-      </c>
-      <c r="F35" s="21">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="19">
+      <c r="A36" s="18">
         <v>20</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>0.21</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="20">
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="G36" s="17" t="s">
-        <v>97</v>
+      <c r="G36" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="19">
+      <c r="A37" s="18">
         <v>20</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="19" t="s">
+      <c r="B37" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E37" s="21">
+      <c r="D37" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="20">
         <v>0.21</v>
       </c>
-      <c r="F37" s="21">
+      <c r="F37" s="20">
         <f t="shared" ref="F37:F38" si="2">A37*E37</f>
         <v>4.2</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="G37" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>20</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="19">
-        <v>20</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="21">
+      <c r="E38" s="20">
         <v>0.18</v>
       </c>
-      <c r="F38" s="21">
+      <c r="F38" s="20">
         <f t="shared" si="2"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="G38" s="17" t="s">
-        <v>97</v>
+      <c r="G38" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="19">
+      <c r="A39" s="18">
         <v>10</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="E39" s="20">
+        <v>11</v>
+      </c>
+      <c r="F39" s="20">
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="E39" s="21">
-        <v>11</v>
-      </c>
-      <c r="F39" s="21">
-        <f t="shared" si="0"/>
+      <c r="G39" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="17" t="s">
+    </row>
+    <row r="40" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="18">
+        <v>10</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="19">
+      <c r="E40" s="20">
+        <v>2.13</v>
+      </c>
+      <c r="F40" s="20">
+        <f t="shared" si="0"/>
+        <v>21.299999999999997</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
         <v>10</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="20" t="s">
+      <c r="B41" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E40" s="21">
-        <v>2.13</v>
-      </c>
-      <c r="F40" s="21">
-        <f t="shared" si="0"/>
-        <v>21.299999999999997</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="19">
-        <v>10</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41" s="21">
+      <c r="E41" s="20">
         <v>1.61</v>
       </c>
-      <c r="F41" s="21">
+      <c r="F41" s="20">
         <f t="shared" si="0"/>
         <v>16.100000000000001</v>
       </c>
-      <c r="G41" s="17" t="s">
-        <v>119</v>
+      <c r="G41" s="16" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1870,20 +1856,20 @@
         <v>3</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" s="13">
+        <v>114</v>
+      </c>
+      <c r="E42" s="12">
         <v>0.95</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="12">
         <f t="shared" ref="F42" si="3">A42*E42</f>
         <v>3.8</v>
       </c>
-      <c r="G42" s="17" t="s">
-        <v>120</v>
+      <c r="G42" s="16" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1894,20 +1880,20 @@
         <v>3</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E43" s="13">
+        <v>116</v>
+      </c>
+      <c r="E43" s="12">
         <v>1.31</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="12">
         <f t="shared" ref="F43" si="4">A43*E43</f>
         <v>5.24</v>
       </c>
-      <c r="G43" s="17" t="s">
-        <v>120</v>
+      <c r="G43" s="16" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1923,10 +1909,10 @@
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="12">
         <v>20.11</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="12">
         <f t="shared" si="0"/>
         <v>40.22</v>
       </c>
@@ -1947,16 +1933,16 @@
       <c r="D45" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="12">
         <v>33.78</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="12">
         <f t="shared" si="0"/>
         <v>168.9</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="8">
+      <c r="A46" s="7">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1966,107 +1952,107 @@
         <v>75</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" s="13">
+        <v>93</v>
+      </c>
+      <c r="E46" s="12">
         <v>49.29</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="12">
         <f t="shared" si="0"/>
         <v>49.29</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="8">
+      <c r="A47" s="7">
         <v>5</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="19" t="s">
+      <c r="B47" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="21">
+      <c r="D47" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="20">
         <v>0.37</v>
       </c>
-      <c r="F47" s="21">
+      <c r="F47" s="20">
         <f t="shared" si="0"/>
         <v>1.85</v>
       </c>
-      <c r="G47" s="17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="25">
+      <c r="G47" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="23">
         <v>1</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="21">
+        <v>14.91</v>
+      </c>
+      <c r="F48" s="21">
+        <f t="shared" si="0"/>
+        <v>14.91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="23">
+        <v>1</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" s="22">
-        <v>14.91</v>
-      </c>
-      <c r="F48" s="22">
-        <f t="shared" si="0"/>
-        <v>14.91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="25">
+      <c r="E49" s="21">
+        <v>14.24</v>
+      </c>
+      <c r="F49" s="21">
+        <f t="shared" si="0"/>
+        <v>14.24</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="23">
         <v>1</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="B50" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D50" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E49" s="22">
+      <c r="E50" s="21">
         <v>14.24</v>
       </c>
-      <c r="F49" s="22">
-        <f t="shared" si="0"/>
-        <v>14.24</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="25">
-        <v>1</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E50" s="22">
-        <v>14.24</v>
-      </c>
-      <c r="F50" s="22">
+      <c r="F50" s="21">
         <f t="shared" ref="F50:F53" si="5">A50*E50</f>
         <v>14.24</v>
       </c>
-      <c r="G50" s="17" t="s">
-        <v>128</v>
+      <c r="G50" s="16" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -2082,10 +2068,10 @@
       <c r="D51" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="12">
         <v>6.34</v>
       </c>
-      <c r="F51" s="13">
+      <c r="F51" s="12">
         <f t="shared" si="5"/>
         <v>31.7</v>
       </c>
@@ -2098,20 +2084,20 @@
         <v>3</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E52" s="13">
+        <v>132</v>
+      </c>
+      <c r="E52" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F52" s="13">
+      <c r="F52" s="12">
         <f t="shared" ref="F52" si="6">A52*E52</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="G52" s="17" t="s">
-        <v>135</v>
+      <c r="G52" s="16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -2121,28 +2107,28 @@
       <c r="B53" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="C53" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="E53" s="13">
+      <c r="E53" s="12">
         <v>14.26</v>
       </c>
-      <c r="F53" s="13">
+      <c r="F53" s="12">
         <f t="shared" si="5"/>
         <v>14.26</v>
       </c>
-      <c r="G53" s="28" t="s">
-        <v>138</v>
+      <c r="G53" s="25" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E55" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="24">
+      <c r="F55" s="26">
         <f>SUM(F4:F53)</f>
         <v>776.12000000000012</v>
       </c>
@@ -2153,10 +2139,10 @@
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E59" s="14"/>
+      <c r="D59" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E59" s="13"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
@@ -2173,10 +2159,10 @@
       <c r="D61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F61" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G61" s="1" t="s">
@@ -2184,99 +2170,97 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="15">
+      <c r="A62" s="14">
         <v>1</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="13">
+      <c r="E62" s="12">
         <v>123.52</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="12">
         <f t="shared" ref="F62:F65" si="7">A62*E62</f>
         <v>123.52</v>
       </c>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="15">
+      <c r="A63" s="14">
         <v>1</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E63" s="12">
         <v>109.24</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="12">
         <f t="shared" si="7"/>
         <v>109.24</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="15">
+      <c r="A64" s="14">
         <v>1</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="12">
         <v>19.920000000000002</v>
       </c>
-      <c r="F64" s="13">
+      <c r="F64" s="12">
         <f t="shared" si="7"/>
         <v>19.920000000000002</v>
       </c>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="15">
+      <c r="A65" s="14">
         <v>1</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E65" s="13">
+      <c r="E65" s="12">
         <v>42.65</v>
       </c>
-      <c r="F65" s="13">
+      <c r="F65" s="12">
         <f t="shared" si="7"/>
         <v>42.65</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="G65" s="3"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E67" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="6">
+      <c r="F67" s="26">
         <f>SUM(F62:F65)</f>
         <v>295.33</v>
       </c>
@@ -2317,26 +2301,26 @@
     <hyperlink ref="C62" r:id="rId32" display="P-T290FX" xr:uid="{E5348CE9-9D00-4F43-BC80-2FA53294A1AC}"/>
     <hyperlink ref="C64" r:id="rId33" xr:uid="{3EBB833A-2474-1B4D-99E1-5DF01289E30B}"/>
     <hyperlink ref="C63" r:id="rId34" xr:uid="{60217A4C-F42A-DE47-8772-D40736914186}"/>
-    <hyperlink ref="G65" r:id="rId35" display="1750a may be suitable?" xr:uid="{45B31A70-473B-674E-94EA-5880AAC62A9F}"/>
-    <hyperlink ref="C27" r:id="rId36" xr:uid="{56C73929-769E-8149-AFDC-F5968AA60469}"/>
-    <hyperlink ref="C47" r:id="rId37" xr:uid="{D9B0D504-B1EF-0B40-B2E4-80C013EAC8D5}"/>
-    <hyperlink ref="C35" r:id="rId38" xr:uid="{79682C29-75D8-2045-971F-EA2196D55BA7}"/>
-    <hyperlink ref="C34" r:id="rId39" xr:uid="{55029CD2-DD3A-FD49-805F-F7C62EF32278}"/>
-    <hyperlink ref="C37" r:id="rId40" xr:uid="{32D2DDE4-B5EE-0748-892A-B34C30E39E4C}"/>
-    <hyperlink ref="C39" r:id="rId41" xr:uid="{36375FE2-CC34-354A-A0F8-BB63F42FA6C1}"/>
-    <hyperlink ref="C36" r:id="rId42" display="S-H172" xr:uid="{EC4736A9-C917-C843-AF22-752E5FEB23DC}"/>
-    <hyperlink ref="C33" r:id="rId43" xr:uid="{2D13C61A-83D2-354C-B62A-0F406A0BACBB}"/>
-    <hyperlink ref="C38" r:id="rId44" xr:uid="{E0709DA1-7F5B-E941-B3EA-65A7D845FEB9}"/>
-    <hyperlink ref="C40" r:id="rId45" xr:uid="{6E8B4E78-80EA-F448-B0A5-F71FB69DFAAB}"/>
-    <hyperlink ref="C41" r:id="rId46" xr:uid="{A54F5635-B66B-8646-8A8C-1EDC2641AC2D}"/>
-    <hyperlink ref="C42" r:id="rId47" xr:uid="{AC9794A3-D0FC-D74A-BF01-58FB4B60F938}"/>
-    <hyperlink ref="C43" r:id="rId48" xr:uid="{08464F23-1C1A-314C-B5F2-FB793CEF457B}"/>
-    <hyperlink ref="C48" r:id="rId49" xr:uid="{6C16B382-89ED-224C-A73B-EAE4D423074F}"/>
-    <hyperlink ref="C50" r:id="rId50" xr:uid="{B07E9DD2-254F-5041-91E4-C6B5A03C14C0}"/>
-    <hyperlink ref="C49" r:id="rId51" xr:uid="{7553A24B-A441-4B46-9CC0-23E4B6600962}"/>
-    <hyperlink ref="C51" r:id="rId52" xr:uid="{D5E216EE-4E4C-3645-846B-40F44565422F}"/>
-    <hyperlink ref="C17" r:id="rId53" display="C-SD1-600" xr:uid="{C8598E26-C21B-4D46-9DFA-0853BA50C6A2}"/>
-    <hyperlink ref="C52" r:id="rId54" xr:uid="{14569396-B101-6945-A1F1-687D5E35B515}"/>
+    <hyperlink ref="C27" r:id="rId35" xr:uid="{56C73929-769E-8149-AFDC-F5968AA60469}"/>
+    <hyperlink ref="C47" r:id="rId36" xr:uid="{D9B0D504-B1EF-0B40-B2E4-80C013EAC8D5}"/>
+    <hyperlink ref="C35" r:id="rId37" xr:uid="{79682C29-75D8-2045-971F-EA2196D55BA7}"/>
+    <hyperlink ref="C34" r:id="rId38" xr:uid="{55029CD2-DD3A-FD49-805F-F7C62EF32278}"/>
+    <hyperlink ref="C37" r:id="rId39" xr:uid="{32D2DDE4-B5EE-0748-892A-B34C30E39E4C}"/>
+    <hyperlink ref="C39" r:id="rId40" xr:uid="{36375FE2-CC34-354A-A0F8-BB63F42FA6C1}"/>
+    <hyperlink ref="C36" r:id="rId41" display="S-H172" xr:uid="{EC4736A9-C917-C843-AF22-752E5FEB23DC}"/>
+    <hyperlink ref="C33" r:id="rId42" xr:uid="{2D13C61A-83D2-354C-B62A-0F406A0BACBB}"/>
+    <hyperlink ref="C38" r:id="rId43" xr:uid="{E0709DA1-7F5B-E941-B3EA-65A7D845FEB9}"/>
+    <hyperlink ref="C40" r:id="rId44" xr:uid="{6E8B4E78-80EA-F448-B0A5-F71FB69DFAAB}"/>
+    <hyperlink ref="C41" r:id="rId45" xr:uid="{A54F5635-B66B-8646-8A8C-1EDC2641AC2D}"/>
+    <hyperlink ref="C42" r:id="rId46" xr:uid="{AC9794A3-D0FC-D74A-BF01-58FB4B60F938}"/>
+    <hyperlink ref="C43" r:id="rId47" xr:uid="{08464F23-1C1A-314C-B5F2-FB793CEF457B}"/>
+    <hyperlink ref="C48" r:id="rId48" xr:uid="{6C16B382-89ED-224C-A73B-EAE4D423074F}"/>
+    <hyperlink ref="C50" r:id="rId49" xr:uid="{B07E9DD2-254F-5041-91E4-C6B5A03C14C0}"/>
+    <hyperlink ref="C49" r:id="rId50" xr:uid="{7553A24B-A441-4B46-9CC0-23E4B6600962}"/>
+    <hyperlink ref="C51" r:id="rId51" xr:uid="{D5E216EE-4E4C-3645-846B-40F44565422F}"/>
+    <hyperlink ref="C17" r:id="rId52" display="C-SD1-600" xr:uid="{C8598E26-C21B-4D46-9DFA-0853BA50C6A2}"/>
+    <hyperlink ref="C52" r:id="rId53" xr:uid="{14569396-B101-6945-A1F1-687D5E35B515}"/>
+    <hyperlink ref="C53" r:id="rId54" xr:uid="{F0DDD149-D39F-F84D-B870-2D49CA3766A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrects reverb transformer. 1750A not 1750B
</commit_message>
<xml_diff>
--- a/BOM/Europe/non-mouser-BOM.xlsx
+++ b/BOM/Europe/non-mouser-BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/dev/git/timrobertson100/steel-string-singer-sn-002/BOM/Europe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC450B47-1E6E-2546-B4BF-3D90C6BBD84C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5EA817-0F1B-BF4C-B8DC-CAE683C75D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7640" yWindow="6500" windowWidth="29040" windowHeight="15840" xr2:uid="{0199555C-9F6B-9B4E-9B9C-1898FA1D406E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -284,9 +284,6 @@
     <t>Choke - Hammond 194B Choke Fender 125C1A / 022699</t>
   </si>
   <si>
-    <t>ha1750b</t>
-  </si>
-  <si>
     <t>SKU 23429</t>
   </si>
   <si>
@@ -462,13 +459,16 @@
   <si>
     <t>SKU 32227</t>
   </si>
+  <si>
+    <t>ha1750a</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -595,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,25 +606,20 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -644,9 +639,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,7 +679,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -790,7 +785,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -932,7 +927,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -942,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBE67D0-6312-A44B-85E3-458F1293B8D9}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,11 +956,11 @@
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="D1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -990,97 +985,97 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>2.33</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <f t="shared" ref="F4:F49" si="0">A4*E4</f>
         <v>2.33</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="9">
+        <v>3.75</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="G5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="12">
-        <v>3.75</v>
-      </c>
-      <c r="F5" s="12">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+      <c r="A6" s="11">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
         <v>90</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="F6" s="12">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>0.3</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1096,10 +1091,10 @@
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="9">
         <v>2.75</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
@@ -1117,10 +1112,10 @@
       <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <v>2.75</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>8.25</v>
       </c>
@@ -1138,10 +1133,10 @@
       <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>2.75</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
@@ -1159,10 +1154,10 @@
       <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="9">
         <v>2.92</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
         <v>2.92</v>
       </c>
@@ -1180,10 +1175,10 @@
       <c r="D12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>3.57</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <f t="shared" si="0"/>
         <v>3.57</v>
       </c>
@@ -1201,10 +1196,10 @@
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <v>0.4</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="9">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
@@ -1225,10 +1220,10 @@
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>1.48</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="9">
         <f t="shared" si="0"/>
         <v>10.36</v>
       </c>
@@ -1246,10 +1241,10 @@
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="9">
         <v>1.48</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="9">
         <f t="shared" si="0"/>
         <v>4.4399999999999995</v>
       </c>
@@ -1267,15 +1262,15 @@
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>1.24</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="9">
         <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1291,10 +1286,10 @@
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="9">
         <v>1.95</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="9">
         <f t="shared" ref="F17" si="1">A17*E17</f>
         <v>11.7</v>
       </c>
@@ -1312,10 +1307,10 @@
       <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>1.89</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="9">
         <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
@@ -1333,10 +1328,10 @@
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="9">
         <v>1.17</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="9">
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
@@ -1354,10 +1349,10 @@
       <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="9">
         <v>4.08</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="9">
         <f t="shared" si="0"/>
         <v>4.08</v>
       </c>
@@ -1378,10 +1373,10 @@
       <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="9">
         <v>4.63</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="9">
         <f t="shared" si="0"/>
         <v>9.26</v>
       </c>
@@ -1399,10 +1394,10 @@
       <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="9">
         <v>3.93</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="9">
         <f t="shared" si="0"/>
         <v>7.86</v>
       </c>
@@ -1420,36 +1415,36 @@
       <c r="D23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="9">
         <v>3.14</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="9">
         <f t="shared" si="0"/>
         <v>9.42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="18">
+    <row r="24" spans="1:7" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="14">
         <v>1</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="16">
         <v>26.41</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="16">
         <f t="shared" si="0"/>
         <v>26.41</v>
       </c>
-      <c r="G24" s="16" t="s">
-        <v>89</v>
+      <c r="G24" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1465,19 +1460,19 @@
       <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="9">
         <v>2.3199999999999998</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="9">
         <f t="shared" si="0"/>
         <v>13.919999999999998</v>
       </c>
-      <c r="G25" s="16" t="s">
-        <v>120</v>
+      <c r="G25" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
+      <c r="A26" s="2">
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1489,10 +1484,10 @@
       <c r="D26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="9">
         <v>5</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1501,27 +1496,27 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="17">
+      <c r="A27" s="14">
         <v>1</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="19" t="s">
+      <c r="B27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="E27" s="16">
+        <v>11.84</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="0"/>
+        <v>11.84</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="E27" s="20">
-        <v>11.84</v>
-      </c>
-      <c r="F27" s="20">
-        <f t="shared" si="0"/>
-        <v>11.84</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1537,10 +1532,10 @@
       <c r="D28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="9">
         <v>2.86</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="9">
         <f t="shared" si="0"/>
         <v>8.58</v>
       </c>
@@ -1558,10 +1553,10 @@
       <c r="D29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="9">
         <v>2.25</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="9">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
@@ -1579,36 +1574,36 @@
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="9">
         <v>2.33</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="9">
         <f t="shared" si="0"/>
         <v>4.66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="18">
+    <row r="31" spans="1:7" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="14">
         <v>2</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="19" t="s">
+      <c r="B31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="16">
         <v>2.5099999999999998</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="16">
         <f t="shared" si="0"/>
         <v>5.0199999999999996</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>89</v>
+      <c r="G31" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1624,10 +1619,10 @@
       <c r="D32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="9">
         <v>49.9</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="9">
         <f t="shared" si="0"/>
         <v>49.9</v>
       </c>
@@ -1640,212 +1635,212 @@
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" s="12">
+        <v>105</v>
+      </c>
+      <c r="E33" s="9">
         <v>0.48</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="16">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="G33" s="16" t="s">
-        <v>103</v>
+      <c r="G33" s="13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="18">
+      <c r="A34" s="14">
         <v>50</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="16">
+        <v>0.13</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="14">
+        <v>50</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" s="20">
-        <v>0.13</v>
-      </c>
-      <c r="F34" s="20">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="18">
-        <v>50</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="E35" s="16">
+        <v>0.12</v>
+      </c>
+      <c r="F35" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G35" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="20">
-        <v>0.12</v>
-      </c>
-      <c r="F35" s="20">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="18">
+      <c r="A36" s="14">
         <v>20</v>
       </c>
-      <c r="B36" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="16">
         <v>0.21</v>
       </c>
-      <c r="F36" s="20">
+      <c r="F36" s="16">
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="G36" s="16" t="s">
-        <v>96</v>
+      <c r="G36" s="13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="18">
+      <c r="A37" s="14">
         <v>20</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="18" t="s">
+      <c r="B37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="20">
+      <c r="D37" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="16">
         <v>0.21</v>
       </c>
-      <c r="F37" s="20">
+      <c r="F37" s="16">
         <f t="shared" ref="F37:F38" si="2">A37*E37</f>
         <v>4.2</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G37" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="14">
+        <v>20</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="18">
-        <v>20</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="20">
+      <c r="E38" s="16">
         <v>0.18</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="16">
         <f t="shared" si="2"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="G38" s="16" t="s">
-        <v>96</v>
+      <c r="G38" s="13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="18">
+      <c r="A39" s="14">
         <v>10</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="E39" s="16">
+        <v>11</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="20">
-        <v>11</v>
-      </c>
-      <c r="F39" s="20">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="40" spans="1:7" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="14">
+        <v>10</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="18">
+      <c r="E40" s="16">
+        <v>2.13</v>
+      </c>
+      <c r="F40" s="16">
+        <f t="shared" si="0"/>
+        <v>21.299999999999997</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="14">
         <v>10</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="19" t="s">
+      <c r="B41" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D40" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="20">
-        <v>2.13</v>
-      </c>
-      <c r="F40" s="20">
-        <f t="shared" si="0"/>
-        <v>21.299999999999997</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="18">
-        <v>10</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E41" s="20">
+      <c r="E41" s="16">
         <v>1.61</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="16">
         <f t="shared" si="0"/>
         <v>16.100000000000001</v>
       </c>
-      <c r="G41" s="16" t="s">
-        <v>118</v>
+      <c r="G41" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1856,20 +1851,20 @@
         <v>3</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" s="12">
+        <v>113</v>
+      </c>
+      <c r="E42" s="9">
         <v>0.95</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="9">
         <f t="shared" ref="F42" si="3">A42*E42</f>
         <v>3.8</v>
       </c>
-      <c r="G42" s="16" t="s">
-        <v>119</v>
+      <c r="G42" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1880,20 +1875,20 @@
         <v>3</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" s="12">
+        <v>115</v>
+      </c>
+      <c r="E43" s="9">
         <v>1.31</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="9">
         <f t="shared" ref="F43" si="4">A43*E43</f>
         <v>5.24</v>
       </c>
-      <c r="G43" s="16" t="s">
-        <v>119</v>
+      <c r="G43" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1909,10 +1904,10 @@
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="9">
         <v>20.11</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44" s="9">
         <f t="shared" si="0"/>
         <v>40.22</v>
       </c>
@@ -1933,10 +1928,10 @@
       <c r="D45" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="9">
         <v>33.78</v>
       </c>
-      <c r="F45" s="12">
+      <c r="F45" s="9">
         <f t="shared" si="0"/>
         <v>168.9</v>
       </c>
@@ -1952,12 +1947,12 @@
         <v>75</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="12">
+        <v>92</v>
+      </c>
+      <c r="E46" s="9">
         <v>49.29</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F46" s="9">
         <f t="shared" si="0"/>
         <v>49.29</v>
       </c>
@@ -1966,93 +1961,93 @@
       <c r="A47" s="7">
         <v>5</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="18" t="s">
+      <c r="B47" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E47" s="20">
+      <c r="D47" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="16">
         <v>0.37</v>
       </c>
-      <c r="F47" s="20">
+      <c r="F47" s="16">
         <f t="shared" si="0"/>
         <v>1.85</v>
       </c>
-      <c r="G47" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="23">
+      <c r="G47" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="11">
         <v>1</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="17">
+        <v>14.91</v>
+      </c>
+      <c r="F48" s="17">
+        <f t="shared" si="0"/>
+        <v>14.91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
+        <v>1</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E48" s="21">
-        <v>14.91</v>
-      </c>
-      <c r="F48" s="21">
-        <f t="shared" si="0"/>
-        <v>14.91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="23">
+      <c r="E49" s="17">
+        <v>14.24</v>
+      </c>
+      <c r="F49" s="17">
+        <f t="shared" si="0"/>
+        <v>14.24</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="11">
         <v>1</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="B50" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D50" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E49" s="21">
+      <c r="E50" s="17">
         <v>14.24</v>
       </c>
-      <c r="F49" s="21">
-        <f t="shared" si="0"/>
-        <v>14.24</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="23">
-        <v>1</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="21">
-        <v>14.24</v>
-      </c>
-      <c r="F50" s="21">
+      <c r="F50" s="17">
         <f t="shared" ref="F50:F53" si="5">A50*E50</f>
         <v>14.24</v>
       </c>
-      <c r="G50" s="16" t="s">
-        <v>127</v>
+      <c r="G50" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -2068,10 +2063,10 @@
       <c r="D51" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E51" s="9">
         <v>6.34</v>
       </c>
-      <c r="F51" s="12">
+      <c r="F51" s="9">
         <f t="shared" si="5"/>
         <v>31.7</v>
       </c>
@@ -2084,20 +2079,20 @@
         <v>3</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E52" s="12">
+        <v>131</v>
+      </c>
+      <c r="E52" s="9">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F52" s="12">
+      <c r="F52" s="9">
         <f t="shared" ref="F52" si="6">A52*E52</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="G52" s="16" t="s">
-        <v>134</v>
+      <c r="G52" s="13" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -2108,27 +2103,27 @@
         <v>3</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="12">
+      <c r="E53" s="9">
         <v>14.26</v>
       </c>
-      <c r="F53" s="12">
+      <c r="F53" s="9">
         <f t="shared" si="5"/>
         <v>14.26</v>
       </c>
-      <c r="G53" s="25" t="s">
-        <v>137</v>
+      <c r="G53" s="20" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E55" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="26">
+      <c r="F55" s="21">
         <f>SUM(F4:F53)</f>
         <v>776.12000000000012</v>
       </c>
@@ -2139,10 +2134,10 @@
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E59" s="13"/>
+      <c r="D59" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="10"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
@@ -2170,87 +2165,87 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="14">
+      <c r="A62" s="11">
         <v>1</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="12">
+      <c r="E62" s="9">
         <v>123.52</v>
       </c>
-      <c r="F62" s="12">
+      <c r="F62" s="9">
         <f t="shared" ref="F62:F65" si="7">A62*E62</f>
         <v>123.52</v>
       </c>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="14">
+      <c r="A63" s="11">
         <v>1</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E63" s="12">
+      <c r="E63" s="9">
         <v>109.24</v>
       </c>
-      <c r="F63" s="12">
+      <c r="F63" s="9">
         <f t="shared" si="7"/>
         <v>109.24</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="14">
+      <c r="A64" s="11">
         <v>1</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E64" s="12">
+      <c r="E64" s="9">
         <v>19.920000000000002</v>
       </c>
-      <c r="F64" s="12">
+      <c r="F64" s="9">
         <f t="shared" si="7"/>
         <v>19.920000000000002</v>
       </c>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="14">
+      <c r="A65" s="11">
         <v>1</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D65" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E65" s="12">
+      <c r="E65" s="9">
         <v>42.65</v>
       </c>
-      <c r="F65" s="12">
+      <c r="F65" s="9">
         <f t="shared" si="7"/>
         <v>42.65</v>
       </c>
@@ -2260,7 +2255,7 @@
       <c r="E67" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="26">
+      <c r="F67" s="21">
         <f>SUM(F62:F65)</f>
         <v>295.33</v>
       </c>

</xml_diff>